<commit_message>
Add nodes and search tree provider - Added nodes - Added serialization of nodes - Added search tree provider for nodes - Added file change tracking
</commit_message>
<xml_diff>
--- a/Personal Portfolio - Time Sheet.xlsx
+++ b/Personal Portfolio - Time Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TeodorVecerdi\Desktop\Development\saxion\unity\personal_portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA544970-8247-461D-B0DF-C3E6B00F2E92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F244B4-2C3E-41D9-B16C-1CC96B2F486C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3075" yWindow="1785" windowWidth="21600" windowHeight="11385" xr2:uid="{3F54F729-53DE-410F-8D1B-12B272360E89}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -62,6 +62,13 @@
 * Set up git repository and Codacy code analysis
 * Researched how ShaderGraph handles some of the things I wanted to implement
 * Set up a Github repository for the project</t>
+  </si>
+  <si>
+    <t>* Added nodes
+* Added node serialization
+* Added Undo/Redo (hopefully) and file change tracking
+* Added search tree for nodes
+* Researched the internals of ShaderGraph to learn how a bunch of things are done there, then reverse-engineered some of them</t>
   </si>
 </sst>
 </file>
@@ -437,7 +444,7 @@
   <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,25 +500,28 @@
       </c>
       <c r="G2" s="2">
         <f>SUM(E2:E1000)</f>
-        <v>0.27986111111111101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.46984953703703691</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44103</v>
       </c>
       <c r="B3" s="2">
-        <v>0</v>
+        <v>0.65844907407407405</v>
       </c>
       <c r="C3" s="2">
-        <v>0</v>
+        <v>0.86927083333333333</v>
       </c>
       <c r="D3" s="2">
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" ref="E3:E58" si="0">C3-B3-D3</f>
-        <v>0</v>
+        <v>0.18998842592592594</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add edges and fix Undo/Redo functionality - Fixed the Undo/Redo functionality - Added node connections (edges) and proper serialization and file persistancy for them - Added the ability to drag an edge/connection from a port and drop it somewhere to create a node
</commit_message>
<xml_diff>
--- a/Personal Portfolio - Time Sheet.xlsx
+++ b/Personal Portfolio - Time Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TeodorVecerdi\Desktop\Development\saxion\unity\personal_portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F244B4-2C3E-41D9-B16C-1CC96B2F486C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC7ADF0-25A9-4C62-B588-1334A5A28A51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3075" yWindow="1785" windowWidth="21600" windowHeight="11385" xr2:uid="{3F54F729-53DE-410F-8D1B-12B272360E89}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -69,6 +69,13 @@
 * Added Undo/Redo (hopefully) and file change tracking
 * Added search tree for nodes
 * Researched the internals of ShaderGraph to learn how a bunch of things are done there, then reverse-engineered some of them</t>
+  </si>
+  <si>
+    <t>* Spent a lot of time fixing the Undo/Redo functionality
+* Spent a bunch more time fixing the Undo/Redo functionality because apparently it's so impossible for my tiny brain to understand that you need to save the Undo state of the object before modifying it, and not afterwards leading to the Undo doing absolutely nothing. :/
+* Researched how ShaderGraph implements some features and reversed engineered that into something that works with my architecture (there are quite a few similar things in the codebase but I never just copy pasted things)
+* Added node connections (edges) and proper serialization and file persistancy for them
+* Added the ability to drag an edge/connection from a port and drop it somewhere to create a node</t>
   </si>
 </sst>
 </file>
@@ -444,10 +451,10 @@
   <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" style="1" customWidth="1"/>
     <col min="2" max="5" width="18.7109375" style="2" customWidth="1"/>
@@ -455,7 +462,7 @@
     <col min="7" max="7" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -500,7 +507,7 @@
       </c>
       <c r="G2" s="2">
         <f>SUM(E2:E1000)</f>
-        <v>0.46984953703703691</v>
+        <v>0.82917824074074065</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -508,58 +515,62 @@
         <v>44103</v>
       </c>
       <c r="B3" s="2">
-        <v>0.65844907407407405</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2">
-        <v>0.86927083333333333</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2">
-        <v>2.0833333333333332E-2</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E58" si="0">C3-B3-D3</f>
-        <v>0.18998842592592594</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <f>C3-B3-D3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44104</v>
       </c>
       <c r="B4" s="2">
-        <v>0</v>
+        <v>0.65844907407407405</v>
       </c>
       <c r="C4" s="2">
-        <v>0</v>
+        <v>0.86927083333333333</v>
       </c>
       <c r="D4" s="2">
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="E4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E4" si="0">C4-B4-D4</f>
+        <v>0.18998842592592594</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44105</v>
       </c>
       <c r="B5" s="2">
-        <v>0</v>
+        <v>0.47126157407407404</v>
       </c>
       <c r="C5" s="2">
-        <v>0</v>
+        <v>0.83059027777777772</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E3:E58" si="1">C5-B5-D5</f>
+        <v>0.35932870370370368</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44106</v>
       </c>
@@ -573,11 +584,12 @@
         <v>0</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44107</v>
       </c>
@@ -591,11 +603,12 @@
         <v>0</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44108</v>
       </c>
@@ -609,11 +622,11 @@
         <v>0</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44109</v>
       </c>
@@ -627,11 +640,11 @@
         <v>0</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44110</v>
       </c>
@@ -645,11 +658,11 @@
         <v>0</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44111</v>
       </c>
@@ -663,11 +676,11 @@
         <v>0</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44112</v>
       </c>
@@ -681,11 +694,11 @@
         <v>0</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44113</v>
       </c>
@@ -699,11 +712,11 @@
         <v>0</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44114</v>
       </c>
@@ -717,11 +730,11 @@
         <v>0</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44115</v>
       </c>
@@ -735,11 +748,11 @@
         <v>0</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44116</v>
       </c>
@@ -753,11 +766,11 @@
         <v>0</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44117</v>
       </c>
@@ -771,11 +784,11 @@
         <v>0</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44118</v>
       </c>
@@ -789,11 +802,11 @@
         <v>0</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44119</v>
       </c>
@@ -807,11 +820,11 @@
         <v>0</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44120</v>
       </c>
@@ -825,11 +838,11 @@
         <v>0</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44121</v>
       </c>
@@ -843,11 +856,11 @@
         <v>0</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44122</v>
       </c>
@@ -861,11 +874,11 @@
         <v>0</v>
       </c>
       <c r="E22" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44123</v>
       </c>
@@ -879,11 +892,11 @@
         <v>0</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44124</v>
       </c>
@@ -897,11 +910,11 @@
         <v>0</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44125</v>
       </c>
@@ -915,11 +928,11 @@
         <v>0</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44126</v>
       </c>
@@ -933,11 +946,11 @@
         <v>0</v>
       </c>
       <c r="E26" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44127</v>
       </c>
@@ -951,11 +964,11 @@
         <v>0</v>
       </c>
       <c r="E27" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44128</v>
       </c>
@@ -969,11 +982,11 @@
         <v>0</v>
       </c>
       <c r="E28" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44129</v>
       </c>
@@ -987,11 +1000,11 @@
         <v>0</v>
       </c>
       <c r="E29" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44130</v>
       </c>
@@ -1005,11 +1018,11 @@
         <v>0</v>
       </c>
       <c r="E30" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44131</v>
       </c>
@@ -1023,11 +1036,11 @@
         <v>0</v>
       </c>
       <c r="E31" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44132</v>
       </c>
@@ -1041,11 +1054,11 @@
         <v>0</v>
       </c>
       <c r="E32" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44133</v>
       </c>
@@ -1059,11 +1072,11 @@
         <v>0</v>
       </c>
       <c r="E33" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44134</v>
       </c>
@@ -1077,11 +1090,11 @@
         <v>0</v>
       </c>
       <c r="E34" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44135</v>
       </c>
@@ -1095,11 +1108,11 @@
         <v>0</v>
       </c>
       <c r="E35" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44136</v>
       </c>
@@ -1113,11 +1126,11 @@
         <v>0</v>
       </c>
       <c r="E36" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44137</v>
       </c>
@@ -1131,11 +1144,11 @@
         <v>0</v>
       </c>
       <c r="E37" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44138</v>
       </c>
@@ -1149,11 +1162,11 @@
         <v>0</v>
       </c>
       <c r="E38" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44139</v>
       </c>
@@ -1167,11 +1180,11 @@
         <v>0</v>
       </c>
       <c r="E39" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44140</v>
       </c>
@@ -1185,11 +1198,11 @@
         <v>0</v>
       </c>
       <c r="E40" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44141</v>
       </c>
@@ -1203,11 +1216,11 @@
         <v>0</v>
       </c>
       <c r="E41" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44142</v>
       </c>
@@ -1221,11 +1234,11 @@
         <v>0</v>
       </c>
       <c r="E42" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44143</v>
       </c>
@@ -1239,11 +1252,11 @@
         <v>0</v>
       </c>
       <c r="E43" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44144</v>
       </c>
@@ -1257,11 +1270,11 @@
         <v>0</v>
       </c>
       <c r="E44" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44145</v>
       </c>
@@ -1275,11 +1288,11 @@
         <v>0</v>
       </c>
       <c r="E45" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44146</v>
       </c>
@@ -1293,11 +1306,11 @@
         <v>0</v>
       </c>
       <c r="E46" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44147</v>
       </c>
@@ -1311,11 +1324,11 @@
         <v>0</v>
       </c>
       <c r="E47" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44148</v>
       </c>
@@ -1329,11 +1342,11 @@
         <v>0</v>
       </c>
       <c r="E48" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44149</v>
       </c>
@@ -1347,11 +1360,11 @@
         <v>0</v>
       </c>
       <c r="E49" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44150</v>
       </c>
@@ -1365,11 +1378,11 @@
         <v>0</v>
       </c>
       <c r="E50" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44151</v>
       </c>
@@ -1383,11 +1396,11 @@
         <v>0</v>
       </c>
       <c r="E51" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44152</v>
       </c>
@@ -1401,11 +1414,11 @@
         <v>0</v>
       </c>
       <c r="E52" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44153</v>
       </c>
@@ -1419,11 +1432,11 @@
         <v>0</v>
       </c>
       <c r="E53" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44154</v>
       </c>
@@ -1437,11 +1450,11 @@
         <v>0</v>
       </c>
       <c r="E54" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44155</v>
       </c>
@@ -1455,11 +1468,11 @@
         <v>0</v>
       </c>
       <c r="E55" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44156</v>
       </c>
@@ -1473,11 +1486,11 @@
         <v>0</v>
       </c>
       <c r="E56" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44157</v>
       </c>
@@ -1491,11 +1504,11 @@
         <v>0</v>
       </c>
       <c r="E57" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44158</v>
       </c>
@@ -1509,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="E58" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Properties (Checks, Triggers and Actors) - Added Properties (the checks & triggers I was talking about, and Actors which are basically a property that  holds which entity owns the dialogue line) - Fixed blackboard: you can now properly delete properties. - Added property (de-)serialization - Added node creation from property (either using the search window provider or by dragging a property from the blackboard)
</commit_message>
<xml_diff>
--- a/Personal Portfolio - Time Sheet.xlsx
+++ b/Personal Portfolio - Time Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TeodorVecerdi\Desktop\Development\saxion\unity\personal_portfolio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\saxion\unity\personal_portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC7ADF0-25A9-4C62-B588-1334A5A28A51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFFD621-2E93-40C8-86EF-94A35D39A2A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="1785" windowWidth="21600" windowHeight="11385" xr2:uid="{3F54F729-53DE-410F-8D1B-12B272360E89}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3F54F729-53DE-410F-8D1B-12B272360E89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -76,6 +76,18 @@
 * Researched how ShaderGraph implements some features and reversed engineered that into something that works with my architecture (there are quite a few similar things in the codebase but I never just copy pasted things)
 * Added node connections (edges) and proper serialization and file persistancy for them
 * Added the ability to drag an edge/connection from a port and drop it somewhere to create a node</t>
+  </si>
+  <si>
+    <t>* Moved graph view into an intermediary visual element that holds everything (toolbar, blackboard etc)
+* Fixed blackboard visibility issue</t>
+  </si>
+  <si>
+    <t>* Added Properties (the checks &amp; triggers I was talking about, and Actors which are basically a property that  holds which entity owns the dialogue line)
+* Fixed blackboard: you can now properly delete properties.
+* Added property (de-)serialization
+* Added node creation from property (either using the search window provider or by dragging a property from the blackboard)
+* Did some more research into GraphView and UIElements.
+* Experimented a bit with writing USS (CSS/UI Styling for UIElements)</t>
   </si>
 </sst>
 </file>
@@ -122,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -134,6 +146,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,7 +464,7 @@
   <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -505,12 +518,12 @@
       <c r="F2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="7">
         <f>SUM(E2:E1000)</f>
-        <v>0.82917824074074065</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1.1501620370370369</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44103</v>
       </c>
@@ -563,7 +576,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" ref="E3:E58" si="1">C5-B5-D5</f>
+        <f t="shared" ref="E5:E58" si="1">C5-B5-D5</f>
         <v>0.35932870370370368</v>
       </c>
       <c r="F5" s="6" t="s">
@@ -575,21 +588,23 @@
         <v>44106</v>
       </c>
       <c r="B6" s="2">
-        <v>0</v>
+        <v>0.42722222222222223</v>
       </c>
       <c r="C6" s="2">
-        <v>0</v>
+        <v>0.49140046296296297</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>6.4178240740740744E-2</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44107</v>
       </c>
@@ -608,7 +623,7 @@
       </c>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44108</v>
       </c>
@@ -626,7 +641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44109</v>
       </c>
@@ -644,7 +659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44110</v>
       </c>
@@ -662,7 +677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44111</v>
       </c>
@@ -680,7 +695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44112</v>
       </c>
@@ -698,7 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44113</v>
       </c>
@@ -716,7 +731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44114</v>
       </c>
@@ -734,7 +749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44115</v>
       </c>
@@ -752,7 +767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44116</v>
       </c>
@@ -770,25 +785,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44117</v>
       </c>
       <c r="B17" s="2">
-        <v>0</v>
+        <v>0.55943287037037037</v>
       </c>
       <c r="C17" s="2">
-        <v>0</v>
+        <v>0.81623842592592588</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.25680555555555551</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44118</v>
       </c>
@@ -806,7 +824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44119</v>
       </c>
@@ -824,7 +842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44120</v>
       </c>
@@ -842,7 +860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44121</v>
       </c>
@@ -860,7 +878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44122</v>
       </c>
@@ -878,7 +896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44123</v>
       </c>
@@ -896,7 +914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44124</v>
       </c>
@@ -914,7 +932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44125</v>
       </c>
@@ -932,7 +950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44126</v>
       </c>
@@ -950,7 +968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44127</v>
       </c>
@@ -968,7 +986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44128</v>
       </c>
@@ -986,7 +1004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44129</v>
       </c>
@@ -1004,7 +1022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44130</v>
       </c>
@@ -1022,7 +1040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44131</v>
       </c>
@@ -1040,7 +1058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44132</v>
       </c>

</xml_diff>

<commit_message>
Begin implementation of Self Dialogue Node - Added "Self" dialogue node for when the player has something to say - Implemented a system to have dynamic ports to a node (because it's needed to allow the user to choose character lines - Fixed an issue where the node would get initialized twice when creating a node while dragging a connection from another node
</commit_message>
<xml_diff>
--- a/Personal Portfolio - Time Sheet.xlsx
+++ b/Personal Portfolio - Time Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\saxion\unity\personal_portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFFD621-2E93-40C8-86EF-94A35D39A2A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A777107C-3C2D-4F3A-96DF-43EBF8C8B6CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3F54F729-53DE-410F-8D1B-12B272360E89}"/>
+    <workbookView xWindow="5085" yWindow="1980" windowWidth="21600" windowHeight="11385" xr2:uid="{3F54F729-53DE-410F-8D1B-12B272360E89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -89,6 +89,12 @@
 * Did some more research into GraphView and UIElements.
 * Experimented a bit with writing USS (CSS/UI Styling for UIElements)</t>
   </si>
+  <si>
+    <t>* Added "Self" dialogue node for when the player has something to say
+* Implemented a system to have dynamic ports to a node (because it's needed to allow the user to choose character lines
+* Added custom styling to node
+* Fixed an issue where the node would get initialized twice when creating a node while dragging a connection from another node</t>
+  </si>
 </sst>
 </file>
 
@@ -134,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -147,6 +153,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,7 +471,7 @@
   <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -520,7 +527,7 @@
       </c>
       <c r="G2" s="7">
         <f>SUM(E2:E1000)</f>
-        <v>1.1501620370370369</v>
+        <v>1.2869560185185183</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -785,7 +792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44117</v>
       </c>
@@ -806,25 +813,29 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44118</v>
       </c>
       <c r="B18" s="2">
-        <v>0</v>
-      </c>
-      <c r="C18" s="2">
-        <v>0</v>
+        <v>0.47899305555555555</v>
+      </c>
+      <c r="C18" s="8">
+        <v>0.77626157407407403</v>
       </c>
       <c r="D18" s="2">
-        <v>0</v>
+        <v>0.16047453703703704</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.13679398148148145</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44119</v>
       </c>
@@ -841,8 +852,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44120</v>
       </c>
@@ -859,8 +871,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44121</v>
       </c>
@@ -878,7 +891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44122</v>
       </c>
@@ -896,7 +909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44123</v>
       </c>
@@ -914,7 +927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44124</v>
       </c>
@@ -932,7 +945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44125</v>
       </c>
@@ -950,7 +963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44126</v>
       </c>
@@ -968,7 +981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44127</v>
       </c>
@@ -986,7 +999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44128</v>
       </c>
@@ -1004,7 +1017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44129</v>
       </c>
@@ -1022,7 +1035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44130</v>
       </c>
@@ -1040,7 +1053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44131</v>
       </c>
@@ -1058,7 +1071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44132</v>
       </c>

</xml_diff>

<commit_message>
Add NPC node, connection validation and begin implementing copy&pasting - Added NPC node - Added node connection validation - Added styling and custom node layouts - Fixed issue where renaming a property would not rename nodes that refer to that property - Started working on copy&paste functionality inside the tool
</commit_message>
<xml_diff>
--- a/Personal Portfolio - Time Sheet.xlsx
+++ b/Personal Portfolio - Time Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\saxion\unity\personal_portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A777107C-3C2D-4F3A-96DF-43EBF8C8B6CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3094820F-3AA6-4435-A479-69B42B96B164}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5085" yWindow="1980" windowWidth="21600" windowHeight="11385" xr2:uid="{3F54F729-53DE-410F-8D1B-12B272360E89}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -94,6 +94,13 @@
 * Implemented a system to have dynamic ports to a node (because it's needed to allow the user to choose character lines
 * Added custom styling to node
 * Fixed an issue where the node would get initialized twice when creating a node while dragging a connection from another node</t>
+  </si>
+  <si>
+    <t>* Added NPC node
+* Added node connection validation
+* Added styling and custom node layouts (UIElements learning)
+* Fixed issue where renaming a property would not rename nodes that refer to that property
+* Started working on copy&amp;paste functionality inside the tool</t>
   </si>
 </sst>
 </file>
@@ -471,7 +478,7 @@
   <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -527,7 +534,7 @@
       </c>
       <c r="G2" s="7">
         <f>SUM(E2:E1000)</f>
-        <v>1.2869560185185183</v>
+        <v>1.4785300925925924</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -840,17 +847,20 @@
         <v>44119</v>
       </c>
       <c r="B19" s="2">
-        <v>0</v>
+        <v>0.47355324074074073</v>
       </c>
       <c r="C19" s="2">
-        <v>0</v>
+        <v>0.6651273148148148</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.19157407407407406</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="G19" s="2"/>
     </row>

</xml_diff>

<commit_message>
Add node styling and fix some bugs - Added per-node styling - Fixed an issue where you could connect two ports more than once (i.e. duplicated edges) - Fixed an issue where search window wouldn't be created properly when dragging from port - Fixed an issue where separators between dialogue lines wouldn't get properly removed when removing the corresponding line
</commit_message>
<xml_diff>
--- a/Personal Portfolio - Time Sheet.xlsx
+++ b/Personal Portfolio - Time Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\saxion\unity\personal_portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEF2068-E7A5-4979-AA26-728727655C40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D04BB5-9B25-48F1-B3E8-57B038AE4D0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5085" yWindow="1980" windowWidth="21600" windowHeight="11385" xr2:uid="{3F54F729-53DE-410F-8D1B-12B272360E89}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -101,6 +101,13 @@
 * Added styling and custom node layouts (UIElements learning)
 * Fixed issue where renaming a property would not rename nodes that refer to that property
 * Started working on copy&amp;paste functionality inside the tool</t>
+  </si>
+  <si>
+    <t>* Finished implementing copy&amp;paste
+* Added per-node styling and other look/layout related things (UIElements learning)
+* Fixed an issue where you could connect two ports more than once (i.e. duplicated edges)
+* Fixed an issue where search window wouldn't be created properly when dragging from port
+* Fixed an issue where separators between dialogue lines wouldn't get properly removed when removing the corresponding line</t>
   </si>
 </sst>
 </file>
@@ -478,15 +485,15 @@
   <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" style="1" customWidth="1"/>
     <col min="2" max="5" width="18.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -534,7 +541,7 @@
       </c>
       <c r="G2" s="7">
         <f>SUM(E2:E1000)</f>
-        <v>1.4785300925925924</v>
+        <v>1.7832291666666664</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -872,14 +879,17 @@
         <v>0.46158564814814818</v>
       </c>
       <c r="C20" s="2">
-        <v>0.46158564814814818</v>
+        <v>0.76628472222222221</v>
       </c>
       <c r="D20" s="2">
         <v>0</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.30469907407407404</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="G20" s="2"/>
     </row>

</xml_diff>

<commit_message>
Fix port capacity bug, improve node styling, start implementing runtime functionality/custom inspector - Added a runtime Dialogue Graph object - Parsed editor data into runtime data (better suited for using in a project) - Fixed an issue where the port capacity was not taken into account (i.e if a port could only accept one connection at a time, the tool would ignore that and default to more than one connection) - Began working on a custom inspector for the runtime monobehaviour - Improved/modified node styling
</commit_message>
<xml_diff>
--- a/Personal Portfolio - Time Sheet.xlsx
+++ b/Personal Portfolio - Time Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\saxion\unity\personal_portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D04BB5-9B25-48F1-B3E8-57B038AE4D0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394E1E49-8C9D-4B34-AF31-0332EE69B183}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="1980" windowWidth="21600" windowHeight="11385" xr2:uid="{3F54F729-53DE-410F-8D1B-12B272360E89}"/>
+    <workbookView xWindow="6300" yWindow="1680" windowWidth="21600" windowHeight="11385" xr2:uid="{3F54F729-53DE-410F-8D1B-12B272360E89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -108,6 +108,13 @@
 * Fixed an issue where you could connect two ports more than once (i.e. duplicated edges)
 * Fixed an issue where search window wouldn't be created properly when dragging from port
 * Fixed an issue where separators between dialogue lines wouldn't get properly removed when removing the corresponding line</t>
+  </si>
+  <si>
+    <t>* Added a runtime Dialogue Graph object
+* Parsed editor data into runtime data (better suited for using in a project)
+* Fixed an issue where the port capacity was not taken into account (i.e if a port could only accept one connection at a time, the tool would ignore that and default to more than one connection)
+* Began working on a custom inspector for the runtime monobehaviour
+* Improved/modified node styling</t>
   </si>
 </sst>
 </file>
@@ -485,7 +492,7 @@
   <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -541,7 +548,7 @@
       </c>
       <c r="G2" s="7">
         <f>SUM(E2:E1000)</f>
-        <v>1.7832291666666664</v>
+        <v>2.2157523148148144</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -893,7 +900,7 @@
       </c>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44121</v>
       </c>
@@ -911,7 +918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44122</v>
       </c>
@@ -929,7 +936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44123</v>
       </c>
@@ -947,7 +954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44124</v>
       </c>
@@ -965,7 +972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44125</v>
       </c>
@@ -983,7 +990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44126</v>
       </c>
@@ -1001,7 +1008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44127</v>
       </c>
@@ -1019,7 +1026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44128</v>
       </c>
@@ -1042,17 +1049,20 @@
         <v>44129</v>
       </c>
       <c r="B29" s="2">
-        <v>0</v>
+        <v>0.40201388888888889</v>
       </c>
       <c r="C29" s="2">
-        <v>0</v>
+        <v>0.84842592592592592</v>
       </c>
       <c r="D29" s="2">
-        <v>0</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="E29" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.43252314814814813</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add runtime implementation and bug fixes - Added runtime tool implementation - Added custom inspector for runtime MonoBehaviour - Added small demo project showcasing the runtime functionality of the tool - Added alerts for graph file being deleted - Added functionality to attempt to recover graph file if it ended up as null - Fixed bug where runtime 'Next' property of Nodes wasn't set properly - Fixed small styling bug
</commit_message>
<xml_diff>
--- a/Personal Portfolio - Time Sheet.xlsx
+++ b/Personal Portfolio - Time Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\saxion\unity\personal_portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394E1E49-8C9D-4B34-AF31-0332EE69B183}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED2BF3A-46BF-4F41-BA91-B9844C9AA1BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6300" yWindow="1680" windowWidth="21600" windowHeight="11385" xr2:uid="{3F54F729-53DE-410F-8D1B-12B272360E89}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -115,6 +115,15 @@
 * Fixed an issue where the port capacity was not taken into account (i.e if a port could only accept one connection at a time, the tool would ignore that and default to more than one connection)
 * Began working on a custom inspector for the runtime monobehaviour
 * Improved/modified node styling</t>
+  </si>
+  <si>
+    <t>* Added runtime tool implementation
+* Added custom inspector for runtime MonoBehaviour
+* Added small demo project showcasing the runtime functionality of the tool
+* Added alerts for graph file being deleted
+* Added functionality to attempt to recover graph file if it ended up as null
+* Fixed bug where runtime 'Next' property of Nodes wasn't set properly
+* Fixed small styling bug</t>
   </si>
 </sst>
 </file>
@@ -492,14 +501,14 @@
   <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" style="1" customWidth="1"/>
     <col min="2" max="5" width="18.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="37.42578125" style="5" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -548,7 +557,7 @@
       </c>
       <c r="G2" s="7">
         <f>SUM(E2:E1000)</f>
-        <v>2.2157523148148144</v>
+        <v>2.9158217592592588</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -619,14 +628,14 @@
         <v>0.42722222222222223</v>
       </c>
       <c r="C6" s="2">
-        <v>0.49140046296296297</v>
+        <v>0.65806712962962965</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="1"/>
-        <v>6.4178240740740744E-2</v>
+        <v>0.23084490740740743</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>10</v>
@@ -864,14 +873,14 @@
         <v>0.47355324074074073</v>
       </c>
       <c r="C19" s="2">
-        <v>0.6651273148148148</v>
+        <v>0.7901273148148148</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" si="1"/>
-        <v>0.19157407407407406</v>
+        <v>0.31657407407407406</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>13</v>
@@ -1055,11 +1064,11 @@
         <v>0.84842592592592592</v>
       </c>
       <c r="D29" s="2">
-        <v>1.3888888888888888E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="E29" s="2">
         <f t="shared" si="1"/>
-        <v>0.43252314814814813</v>
+        <v>0.42557870370370371</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>15</v>
@@ -1070,17 +1079,20 @@
         <v>44130</v>
       </c>
       <c r="B30" s="2">
-        <v>0</v>
+        <v>0.38245370370370368</v>
       </c>
       <c r="C30" s="2">
-        <v>0</v>
+        <v>0.79780092592592589</v>
       </c>
       <c r="D30" s="2">
         <v>0</v>
       </c>
       <c r="E30" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.4153472222222222</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>